<commit_message>
ui claim verfied date import does fs changes
</commit_message>
<xml_diff>
--- a/public/documents/trainee_ui_claim_verification_template.xlsx
+++ b/public/documents/trainee_ui_claim_verification_template.xlsx
@@ -17,12 +17,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
     <t>tapo_id</t>
   </si>
   <si>
     <t>ui_claim_verified_on</t>
+  </si>
+  <si>
+    <t>funding_source</t>
   </si>
   <si>
     <t>NC</t>
@@ -32,10 +35,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="GENERAL" numFmtId="165"/>
-    <numFmt formatCode="M/D/YYYY" numFmtId="166"/>
+    <numFmt formatCode="M/D/YYYY" numFmtId="165"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -113,16 +115,17 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="4" numFmtId="165">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="4" numFmtId="164">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="20"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="166" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="20"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="20"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="20"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="165" xfId="20"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -131,7 +134,7 @@
     <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Normal" xfId="20"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Normal" xfId="20"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -141,46 +144,53 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="C3" activeCellId="0" pane="topLeft" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6941176470588"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.278431372549"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.3843137254902"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.9960784313726"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="11.7490196078431"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="2">
-      <c r="A2" s="2" t="n">
+      <c r="A2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="3">
-      <c r="A3" s="2" t="n">
+      <c r="A3" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="n">
+      <c r="B3" s="4" t="n">
         <v>41721</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="4">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>2</v>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -206,7 +216,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="11.7490196078431"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -231,7 +241,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="11.7490196078431"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
disabled is a seperate input column
</commit_message>
<xml_diff>
--- a/public/documents/trainee_ui_claim_verification_template.xlsx
+++ b/public/documents/trainee_ui_claim_verification_template.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>tapo_id</t>
   </si>
@@ -28,16 +28,26 @@
     <t>funding_source</t>
   </si>
   <si>
+    <t>disable</t>
+  </si>
+  <si>
     <t>NC</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
     <numFmt formatCode="M/D/YYYY" numFmtId="165"/>
+    <numFmt formatCode="MM/DD/YY" numFmtId="166"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -120,12 +130,13 @@
       <protection hidden="false" locked="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="20"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="20"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="20"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="165" xfId="20"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="166" xfId="20"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -134,7 +145,7 @@
     <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Normal" xfId="20"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Normal" xfId="20"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -144,17 +155,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100">
-      <selection activeCell="C3" activeCellId="0" pane="topLeft" sqref="C3"/>
+      <selection activeCell="B5" activeCellId="0" pane="topLeft" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.7490196078431"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.3843137254902"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.9960784313726"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.8117647058824"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.4862745098039"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.0745098039216"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="11.8117647058824"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="1">
@@ -167,6 +178,9 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="2">
       <c r="A2" s="3" t="n">
@@ -174,7 +188,10 @@
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="3">
@@ -184,13 +201,19 @@
       <c r="B3" s="4" t="n">
         <v>41721</v>
       </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="4">
       <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
+      <c r="B4" s="5" t="n">
+        <v>41934</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -216,7 +239,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="11.8117647058824"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -241,7 +264,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="11.8117647058824"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>